<commit_message>
BT Sáng 25/6 còn thiếu Edit Delete, tiếp tục làm tiếp.
</commit_message>
<xml_diff>
--- a/PHP-Course/BackEnd-PHP/Ch-03.xlsx
+++ b/PHP-Course/BackEnd-PHP/Ch-03.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="PHP Files" sheetId="13" r:id="rId1"/>
@@ -674,7 +674,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -709,7 +709,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -920,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1773,8 +1773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Đang làm lại BT trên lớp
</commit_message>
<xml_diff>
--- a/PHP-Course/BackEnd-PHP/Ch-03.xlsx
+++ b/PHP-Course/BackEnd-PHP/Ch-03.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="94">
   <si>
     <t>Ktra tình trạng của thư mục = Mảng Array</t>
   </si>
@@ -437,9 +437,6 @@
     <t>    $(document).ready(function(){</t>
   </si>
   <si>
-    <t>        $('#cancel-button').click(function(){</t>
-  </si>
-  <si>
     <t>            window.location = 'index.php';</t>
   </si>
   <si>
@@ -456,6 +453,51 @@
   </si>
   <si>
     <t>Kéo file function.php chứa các hàm mình sử dụng vào file PHP</t>
+  </si>
+  <si>
+    <t>&lt;script type="text/javascript"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/script&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t>        $('#</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>cancel-button</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>').</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>click(function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(){</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -621,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -655,7 +697,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,7 +811,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -800,7 +846,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1206,72 +1252,151 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A15:J26"/>
+  <dimension ref="A15:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>83</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A19" s="3" t="s">
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A20" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H20" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="11"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="11"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="11"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="11"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="11"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="13"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>